<commit_message>
Updated texts for screenshots
</commit_message>
<xml_diff>
--- a/_templates/Edge-Barcode-Scanner-Info/Jobs_Positions_de.xlsx
+++ b/_templates/Edge-Barcode-Scanner-Info/Jobs_Positions_de.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Edge-Barcode-Scanner-Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B9420D-AEFA-5B4B-A01F-2237D38EEFE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC5A033-73E2-F84A-A3AF-654958DF76B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30160" yWindow="2840" windowWidth="20420" windowHeight="25960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>Schinken - gekocht</t>
   </si>
   <si>
-    <t>Rosmarin - Primerba, Paste</t>
-  </si>
-  <si>
     <t>Kalbfleisch - Nuckle</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>Zitronenmelisse - Frisch</t>
   </si>
   <si>
-    <t>Wäscherei - Taschentuch</t>
-  </si>
-  <si>
     <t>Käse - Ermite Bleu</t>
   </si>
   <si>
@@ -187,9 +181,6 @@
     <t>Jakobsmuscheln - 10/20</t>
   </si>
   <si>
-    <t>Brust, Flügel an</t>
-  </si>
-  <si>
     <t>Teller</t>
   </si>
   <si>
@@ -221,6 +212,15 @@
   </si>
   <si>
     <t>danger</t>
+  </si>
+  <si>
+    <t>Brust, Geflügel</t>
+  </si>
+  <si>
+    <t>Rosmarin</t>
+  </si>
+  <si>
+    <t>Taschentücher</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:G868"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -594,10 +594,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -609,10 +609,10 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -626,10 +626,10 @@
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -649,7 +649,7 @@
         <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -672,10 +672,10 @@
         <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -744,7 +744,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -787,7 +787,7 @@
         <v>300</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -810,10 +810,10 @@
         <v>300</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -833,10 +833,10 @@
         <v>300</v>
       </c>
       <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" t="s">
         <v>64</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -856,10 +856,10 @@
         <v>300</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -879,10 +879,10 @@
         <v>300</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13">
         <v>3</v>
@@ -902,10 +902,10 @@
         <v>300</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14">
         <v>2</v>
@@ -925,10 +925,10 @@
         <v>300</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <v>2</v>
@@ -948,10 +948,10 @@
         <v>300</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F16">
         <v>2</v>
@@ -971,10 +971,10 @@
         <v>100</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -997,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -1020,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19">
         <v>5</v>
@@ -1043,7 +1043,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20">
         <v>6</v>
@@ -1063,10 +1063,10 @@
         <v>300</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F21">
         <v>2</v>
@@ -1086,10 +1086,10 @@
         <v>300</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F22">
         <v>3</v>
@@ -1109,10 +1109,10 @@
         <v>300</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1132,10 +1132,10 @@
         <v>300</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24">
         <v>2</v>
@@ -1155,10 +1155,10 @@
         <v>100</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F25">
         <v>4</v>
@@ -1178,10 +1178,10 @@
         <v>100</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E26" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="F26">
         <v>5</v>
@@ -1201,10 +1201,10 @@
         <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F27">
         <v>4</v>
@@ -1224,10 +1224,10 @@
         <v>100</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F28">
         <v>6</v>
@@ -1247,10 +1247,10 @@
         <v>100</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F29">
         <v>4</v>
@@ -1270,10 +1270,10 @@
         <v>100</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F30">
         <v>4</v>
@@ -1293,10 +1293,10 @@
         <v>100</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F31">
         <v>2</v>
@@ -1319,7 +1319,7 @@
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F32">
         <v>3</v>
@@ -1342,7 +1342,7 @@
         <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F33">
         <v>4</v>
@@ -1365,7 +1365,7 @@
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F34">
         <v>5</v>
@@ -1388,7 +1388,7 @@
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F35">
         <v>6</v>
@@ -1408,10 +1408,10 @@
         <v>300</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1431,10 +1431,10 @@
         <v>300</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F37">
         <v>2</v>
@@ -1454,10 +1454,10 @@
         <v>300</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -1477,10 +1477,10 @@
         <v>300</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F39">
         <v>3</v>
@@ -1500,10 +1500,10 @@
         <v>100</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F40">
         <v>4</v>
@@ -1526,7 +1526,7 @@
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F41">
         <v>6</v>
@@ -1549,7 +1549,7 @@
         <v>2</v>
       </c>
       <c r="E42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1572,7 +1572,7 @@
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F43">
         <v>2</v>
@@ -1592,10 +1592,10 @@
         <v>300</v>
       </c>
       <c r="D44" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F44">
         <v>4</v>
@@ -1615,10 +1615,10 @@
         <v>300</v>
       </c>
       <c r="D45" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F45">
         <v>2</v>
@@ -1638,10 +1638,10 @@
         <v>300</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -1661,10 +1661,10 @@
         <v>300</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F47">
         <v>2</v>
@@ -1684,10 +1684,10 @@
         <v>300</v>
       </c>
       <c r="D48" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -1707,10 +1707,10 @@
         <v>300</v>
       </c>
       <c r="D49" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F49">
         <v>2</v>
@@ -1730,10 +1730,10 @@
         <v>300</v>
       </c>
       <c r="D50" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F50">
         <v>2</v>
@@ -1753,10 +1753,10 @@
         <v>300</v>
       </c>
       <c r="D51" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -1776,10 +1776,10 @@
         <v>100</v>
       </c>
       <c r="D52" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E52" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -1799,10 +1799,10 @@
         <v>100</v>
       </c>
       <c r="D53" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F53">
         <v>3</v>
@@ -1822,10 +1822,10 @@
         <v>100</v>
       </c>
       <c r="D54" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E54" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F54">
         <v>4</v>
@@ -1845,10 +1845,10 @@
         <v>100</v>
       </c>
       <c r="D55" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E55" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F55">
         <v>5</v>
@@ -1868,10 +1868,10 @@
         <v>100</v>
       </c>
       <c r="D56" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E56" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F56">
         <v>6</v>
@@ -1894,7 +1894,7 @@
         <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F57">
         <v>4</v>
@@ -1917,7 +1917,7 @@
         <v>2</v>
       </c>
       <c r="E58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F58">
         <v>2</v>
@@ -1940,7 +1940,7 @@
         <v>2</v>
       </c>
       <c r="E59" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -1960,10 +1960,10 @@
         <v>300</v>
       </c>
       <c r="D60" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E60" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F60">
         <v>4</v>
@@ -1983,10 +1983,10 @@
         <v>300</v>
       </c>
       <c r="D61" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E61" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F61">
         <v>1</v>

</xml_diff>